<commit_message>
corrected how KCmultiply deals with termination impedances. added allertonproc.cls.
</commit_message>
<xml_diff>
--- a/how partialcells should operate.xlsx
+++ b/how partialcells should operate.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13260" yWindow="460" windowWidth="20960" windowHeight="15240" tabRatio="500"/>
+    <workbookView xWindow="3260" yWindow="460" windowWidth="20960" windowHeight="15240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="20">
   <si>
     <t>ABCDgaphalf2</t>
   </si>
@@ -75,6 +75,18 @@
   </si>
   <si>
     <t>%then the antenna ends above a gap in the middle layer - is this connection ok in the top layer?</t>
+  </si>
+  <si>
+    <t>rest of cells</t>
+  </si>
+  <si>
+    <t>cell except gap cap at end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number of unit cells not under antenna on ONE HALF of substrate: floor((L_sub-L_ant)/2)-1 </t>
+  </si>
+  <si>
+    <t>(the -1 is because the edge isn't going to behave like a full unit cell - it's a microstrip open rather than a gap cap)</t>
   </si>
 </sst>
 </file>
@@ -413,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:H29"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -424,17 +436,27 @@
     <col min="6" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>7</v>
       </c>
@@ -442,7 +464,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
         <v>2</v>
       </c>
@@ -456,15 +478,21 @@
         <v>0</v>
       </c>
       <c r="G7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>7</v>
       </c>
@@ -475,7 +503,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D13" t="s">
         <v>4</v>
       </c>
@@ -489,15 +517,21 @@
         <v>0</v>
       </c>
       <c r="H13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J13" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>7</v>
       </c>
@@ -511,7 +545,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="E18" t="s">
         <v>2</v>
       </c>
@@ -519,15 +553,21 @@
         <v>0</v>
       </c>
       <c r="G18" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18" t="s">
+        <v>17</v>
+      </c>
+      <c r="I18" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>7</v>
       </c>
@@ -544,7 +584,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="F24" t="s">
         <v>4</v>
       </c>
@@ -552,15 +592,21 @@
         <v>0</v>
       </c>
       <c r="H24" t="s">
+        <v>16</v>
+      </c>
+      <c r="I24" t="s">
+        <v>17</v>
+      </c>
+      <c r="J24" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>7</v>
       </c>
@@ -580,11 +626,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="G29" t="s">
         <v>0</v>
       </c>
       <c r="H29" t="s">
+        <v>16</v>
+      </c>
+      <c r="I29" t="s">
+        <v>17</v>
+      </c>
+      <c r="J29" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>